<commit_message>
a mightly long way to appease stickler
</commit_message>
<xml_diff>
--- a/tests/data/testing_metadata.xlsx
+++ b/tests/data/testing_metadata.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dh/Github/pyam/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E09F7E4-CE68-0145-A516-DF4FEBEADDBF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F368239-8AAC-F247-880B-35B61B8561F0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="16380" windowHeight="8200" tabRatio="993" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" iterateDelta="1E-4"/>
+  <calcPr calcId="181029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -39,16 +39,16 @@
     <t>category</t>
   </si>
   <si>
-    <t>a_model</t>
-  </si>
-  <si>
-    <t>a_scenario</t>
-  </si>
-  <si>
     <t>imported</t>
   </si>
   <si>
-    <t>a_scenario3</t>
+    <t>model_a</t>
+  </si>
+  <si>
+    <t>scen_a</t>
+  </si>
+  <si>
+    <t>scen_c</t>
   </si>
 </sst>
 </file>
@@ -429,7 +429,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -456,22 +456,22 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" t="b">
         <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
@@ -481,7 +481,7 @@
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>